<commit_message>
Updated legend to include the negative and positive indicators for "No Smoothing"
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -434,6 +434,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Unnamed: 0</t>
@@ -456,7 +461,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
@@ -473,7 +478,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="n">
@@ -490,7 +495,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="A4" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="n">
@@ -507,7 +512,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="n">
@@ -524,7 +529,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="n">
@@ -541,7 +546,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="n">
@@ -558,7 +563,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="n">
@@ -575,7 +580,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" t="n">
         <v>7</v>
       </c>
       <c r="B9" t="n">
@@ -592,7 +597,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" t="n">
         <v>8</v>
       </c>
       <c r="B10" t="n">
@@ -609,7 +614,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
+      <c r="A11" t="n">
         <v>9</v>
       </c>
       <c r="B11" t="n">
@@ -626,7 +631,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
+      <c r="A12" t="n">
         <v>10</v>
       </c>
       <c r="B12" t="n">
@@ -643,7 +648,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
+      <c r="A13" t="n">
         <v>11</v>
       </c>
       <c r="B13" t="n">
@@ -660,7 +665,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
+      <c r="A14" t="n">
         <v>12</v>
       </c>
       <c r="B14" t="n">
@@ -677,7 +682,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
+      <c r="A15" t="n">
         <v>13</v>
       </c>
       <c r="B15" t="n">
@@ -694,7 +699,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
+      <c r="A16" t="n">
         <v>14</v>
       </c>
       <c r="B16" t="n">
@@ -711,7 +716,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n">
+      <c r="A17" t="n">
         <v>15</v>
       </c>
       <c r="B17" t="n">
@@ -728,7 +733,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n">
+      <c r="A18" t="n">
         <v>16</v>
       </c>
       <c r="B18" t="n">
@@ -745,7 +750,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n">
+      <c r="A19" t="n">
         <v>17</v>
       </c>
       <c r="B19" t="n">
@@ -762,7 +767,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
+      <c r="A20" t="n">
         <v>18</v>
       </c>
       <c r="B20" t="n">
@@ -779,7 +784,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="n">
+      <c r="A21" t="n">
         <v>19</v>
       </c>
       <c r="B21" t="n">
@@ -796,7 +801,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="n">
+      <c r="A22" t="n">
         <v>20</v>
       </c>
       <c r="B22" t="n">
@@ -813,7 +818,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="n">
+      <c r="A23" t="n">
         <v>21</v>
       </c>
       <c r="B23" t="n">
@@ -830,7 +835,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="n">
+      <c r="A24" t="n">
         <v>22</v>
       </c>
       <c r="B24" t="n">
@@ -847,7 +852,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="n">
+      <c r="A25" t="n">
         <v>23</v>
       </c>
       <c r="B25" t="n">
@@ -864,7 +869,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="n">
+      <c r="A26" t="n">
         <v>24</v>
       </c>
       <c r="B26" t="n">
@@ -881,7 +886,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="n">
+      <c r="A27" t="n">
         <v>25</v>
       </c>
       <c r="B27" t="n">
@@ -898,7 +903,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="n">
+      <c r="A28" t="n">
         <v>26</v>
       </c>
       <c r="B28" t="n">
@@ -915,7 +920,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="n">
+      <c r="A29" t="n">
         <v>27</v>
       </c>
       <c r="B29" t="n">
@@ -932,7 +937,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="n">
+      <c r="A30" t="n">
         <v>28</v>
       </c>
       <c r="B30" t="n">
@@ -949,7 +954,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="n">
+      <c r="A31" t="n">
         <v>29</v>
       </c>
       <c r="B31" t="n">
@@ -966,7 +971,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="n">
+      <c r="A32" t="n">
         <v>30</v>
       </c>
       <c r="B32" t="n">
@@ -983,7 +988,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="n">
+      <c r="A33" t="n">
         <v>31</v>
       </c>
       <c r="B33" t="n">
@@ -1000,7 +1005,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="n">
+      <c r="A34" t="n">
         <v>32</v>
       </c>
       <c r="B34" t="n">
@@ -1017,7 +1022,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="n">
+      <c r="A35" t="n">
         <v>33</v>
       </c>
       <c r="B35" t="n">
@@ -1034,7 +1039,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="n">
+      <c r="A36" t="n">
         <v>34</v>
       </c>
       <c r="B36" t="n">
@@ -1051,7 +1056,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="n">
+      <c r="A37" t="n">
         <v>35</v>
       </c>
       <c r="B37" t="n">
@@ -1068,7 +1073,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="n">
+      <c r="A38" t="n">
         <v>36</v>
       </c>
       <c r="B38" t="n">
@@ -1085,7 +1090,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="n">
+      <c r="A39" t="n">
         <v>37</v>
       </c>
       <c r="B39" t="n">
@@ -1102,7 +1107,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="n">
+      <c r="A40" t="n">
         <v>38</v>
       </c>
       <c r="B40" t="n">
@@ -1119,7 +1124,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="n">
+      <c r="A41" t="n">
         <v>39</v>
       </c>
       <c r="B41" t="n">
@@ -1136,7 +1141,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="n">
+      <c r="A42" t="n">
         <v>40</v>
       </c>
       <c r="B42" t="n">
@@ -1153,7 +1158,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="n">
+      <c r="A43" t="n">
         <v>41</v>
       </c>
       <c r="B43" t="n">
@@ -1170,7 +1175,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="n">
+      <c r="A44" t="n">
         <v>42</v>
       </c>
       <c r="B44" t="n">
@@ -1187,7 +1192,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="n">
+      <c r="A45" t="n">
         <v>43</v>
       </c>
       <c r="B45" t="n">
@@ -1204,7 +1209,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="n">
+      <c r="A46" t="n">
         <v>44</v>
       </c>
       <c r="B46" t="n">
@@ -1221,7 +1226,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="n">
+      <c r="A47" t="n">
         <v>45</v>
       </c>
       <c r="B47" t="n">
@@ -1238,7 +1243,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="n">
+      <c r="A48" t="n">
         <v>46</v>
       </c>
       <c r="B48" t="n">
@@ -1255,7 +1260,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="n">
+      <c r="A49" t="n">
         <v>47</v>
       </c>
       <c r="B49" t="n">
@@ -1272,7 +1277,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="n">
+      <c r="A50" t="n">
         <v>48</v>
       </c>
       <c r="B50" t="n">
@@ -1289,7 +1294,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="n">
+      <c r="A51" t="n">
         <v>49</v>
       </c>
       <c r="B51" t="n">
@@ -1306,7 +1311,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="n">
+      <c r="A52" t="n">
         <v>50</v>
       </c>
       <c r="B52" t="n">
@@ -1323,7 +1328,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="n">
+      <c r="A53" t="n">
         <v>51</v>
       </c>
       <c r="B53" t="n">
@@ -1340,7 +1345,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="n">
+      <c r="A54" t="n">
         <v>52</v>
       </c>
       <c r="B54" t="n">
@@ -1357,7 +1362,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="n">
+      <c r="A55" t="n">
         <v>53</v>
       </c>
       <c r="B55" t="n">
@@ -1374,7 +1379,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="n">
+      <c r="A56" t="n">
         <v>54</v>
       </c>
       <c r="B56" t="n">
@@ -1391,7 +1396,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="n">
+      <c r="A57" t="n">
         <v>55</v>
       </c>
       <c r="B57" t="n">
@@ -1408,7 +1413,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="n">
+      <c r="A58" t="n">
         <v>56</v>
       </c>
       <c r="B58" t="n">
@@ -1425,7 +1430,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="1" t="n">
+      <c r="A59" t="n">
         <v>57</v>
       </c>
       <c r="B59" t="n">
@@ -1442,7 +1447,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="n">
+      <c r="A60" t="n">
         <v>58</v>
       </c>
       <c r="B60" t="n">
@@ -1459,7 +1464,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="n">
+      <c r="A61" t="n">
         <v>59</v>
       </c>
       <c r="B61" t="n">
@@ -1476,7 +1481,7 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="n">
+      <c r="A62" t="n">
         <v>60</v>
       </c>
       <c r="B62" t="n">
@@ -1493,7 +1498,7 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="n">
+      <c r="A63" t="n">
         <v>61</v>
       </c>
       <c r="B63" t="n">
@@ -1510,7 +1515,7 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="1" t="n">
+      <c r="A64" t="n">
         <v>62</v>
       </c>
       <c r="B64" t="n">
@@ -1527,7 +1532,7 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="1" t="n">
+      <c r="A65" t="n">
         <v>63</v>
       </c>
       <c r="B65" t="n">
@@ -1544,7 +1549,7 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="1" t="n">
+      <c r="A66" t="n">
         <v>64</v>
       </c>
       <c r="B66" t="n">
@@ -1561,7 +1566,7 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="n">
+      <c r="A67" t="n">
         <v>65</v>
       </c>
       <c r="B67" t="n">
@@ -1578,7 +1583,7 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="1" t="n">
+      <c r="A68" t="n">
         <v>66</v>
       </c>
       <c r="B68" t="n">
@@ -1595,7 +1600,7 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="1" t="n">
+      <c r="A69" t="n">
         <v>67</v>
       </c>
       <c r="B69" t="n">
@@ -1612,7 +1617,7 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="1" t="n">
+      <c r="A70" t="n">
         <v>68</v>
       </c>
       <c r="B70" t="n">
@@ -1629,7 +1634,7 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="1" t="n">
+      <c r="A71" t="n">
         <v>69</v>
       </c>
       <c r="B71" t="n">
@@ -1646,7 +1651,7 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="1" t="n">
+      <c r="A72" t="n">
         <v>70</v>
       </c>
       <c r="B72" t="n">
@@ -1663,7 +1668,7 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="1" t="n">
+      <c r="A73" t="n">
         <v>71</v>
       </c>
       <c r="B73" t="n">
@@ -1680,7 +1685,7 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="1" t="n">
+      <c r="A74" t="n">
         <v>72</v>
       </c>
       <c r="B74" t="n">
@@ -1697,7 +1702,7 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="1" t="n">
+      <c r="A75" t="n">
         <v>73</v>
       </c>
       <c r="B75" t="n">
@@ -1714,7 +1719,7 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="1" t="n">
+      <c r="A76" t="n">
         <v>74</v>
       </c>
       <c r="B76" t="n">
@@ -1731,7 +1736,7 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="1" t="n">
+      <c r="A77" t="n">
         <v>75</v>
       </c>
       <c r="B77" t="n">
@@ -1748,7 +1753,7 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="1" t="n">
+      <c r="A78" t="n">
         <v>76</v>
       </c>
       <c r="B78" t="n">
@@ -1765,7 +1770,7 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="1" t="n">
+      <c r="A79" t="n">
         <v>77</v>
       </c>
       <c r="B79" t="n">
@@ -1782,7 +1787,7 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="1" t="n">
+      <c r="A80" t="n">
         <v>78</v>
       </c>
       <c r="B80" t="n">
@@ -1799,7 +1804,7 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="1" t="n">
+      <c r="A81" t="n">
         <v>79</v>
       </c>
       <c r="B81" t="n">
@@ -1816,7 +1821,7 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="1" t="n">
+      <c r="A82" t="n">
         <v>80</v>
       </c>
       <c r="B82" t="n">
@@ -1833,7 +1838,7 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="1" t="n">
+      <c r="A83" t="n">
         <v>81</v>
       </c>
       <c r="B83" t="n">
@@ -1850,7 +1855,7 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="1" t="n">
+      <c r="A84" t="n">
         <v>82</v>
       </c>
       <c r="B84" t="n">
@@ -1867,7 +1872,7 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="1" t="n">
+      <c r="A85" t="n">
         <v>83</v>
       </c>
       <c r="B85" t="n">
@@ -1884,7 +1889,7 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="1" t="n">
+      <c r="A86" t="n">
         <v>84</v>
       </c>
       <c r="B86" t="n">
@@ -1901,7 +1906,7 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="1" t="n">
+      <c r="A87" t="n">
         <v>85</v>
       </c>
       <c r="B87" t="n">
@@ -1918,7 +1923,7 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="1" t="n">
+      <c r="A88" t="n">
         <v>86</v>
       </c>
       <c r="B88" t="n">
@@ -1935,7 +1940,7 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="1" t="n">
+      <c r="A89" t="n">
         <v>87</v>
       </c>
       <c r="B89" t="n">
@@ -1952,7 +1957,7 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="1" t="n">
+      <c r="A90" t="n">
         <v>88</v>
       </c>
       <c r="B90" t="n">
@@ -1969,7 +1974,7 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="1" t="n">
+      <c r="A91" t="n">
         <v>89</v>
       </c>
       <c r="B91" t="n">
@@ -1986,7 +1991,7 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="1" t="n">
+      <c r="A92" t="n">
         <v>90</v>
       </c>
       <c r="B92" t="n">
@@ -2003,7 +2008,7 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="1" t="n">
+      <c r="A93" t="n">
         <v>91</v>
       </c>
       <c r="B93" t="n">
@@ -2020,7 +2025,7 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="1" t="n">
+      <c r="A94" t="n">
         <v>92</v>
       </c>
       <c r="B94" t="n">
@@ -2037,7 +2042,7 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="1" t="n">
+      <c r="A95" t="n">
         <v>93</v>
       </c>
       <c r="B95" t="n">
@@ -2054,7 +2059,7 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="1" t="n">
+      <c r="A96" t="n">
         <v>94</v>
       </c>
       <c r="B96" t="n">
@@ -2071,7 +2076,7 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="1" t="n">
+      <c r="A97" t="n">
         <v>95</v>
       </c>
       <c r="B97" t="n">
@@ -2088,7 +2093,7 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="1" t="n">
+      <c r="A98" t="n">
         <v>96</v>
       </c>
       <c r="B98" t="n">
@@ -2105,7 +2110,7 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="1" t="n">
+      <c r="A99" t="n">
         <v>97</v>
       </c>
       <c r="B99" t="n">
@@ -2122,7 +2127,7 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="1" t="n">
+      <c r="A100" t="n">
         <v>98</v>
       </c>
       <c r="B100" t="n">
@@ -2139,7 +2144,7 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="1" t="n">
+      <c r="A101" t="n">
         <v>99</v>
       </c>
       <c r="B101" t="n">
@@ -2156,7 +2161,7 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="1" t="n">
+      <c r="A102" t="n">
         <v>100</v>
       </c>
       <c r="B102" t="n">
@@ -2173,7 +2178,7 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="1" t="n">
+      <c r="A103" t="n">
         <v>101</v>
       </c>
       <c r="B103" t="n">
@@ -2190,7 +2195,7 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="1" t="n">
+      <c r="A104" t="n">
         <v>102</v>
       </c>
       <c r="B104" t="n">
@@ -2207,7 +2212,7 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="1" t="n">
+      <c r="A105" t="n">
         <v>103</v>
       </c>
       <c r="B105" t="n">
@@ -2224,7 +2229,7 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="1" t="n">
+      <c r="A106" t="n">
         <v>104</v>
       </c>
       <c r="B106" t="n">
@@ -2241,7 +2246,7 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="1" t="n">
+      <c r="A107" t="n">
         <v>105</v>
       </c>
       <c r="B107" t="n">
@@ -2258,7 +2263,7 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="1" t="n">
+      <c r="A108" t="n">
         <v>106</v>
       </c>
       <c r="B108" t="n">
@@ -2275,7 +2280,7 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="1" t="n">
+      <c r="A109" t="n">
         <v>107</v>
       </c>
       <c r="B109" t="n">
@@ -2292,7 +2297,7 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="1" t="n">
+      <c r="A110" t="n">
         <v>108</v>
       </c>
       <c r="B110" t="n">
@@ -2309,7 +2314,7 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="1" t="n">
+      <c r="A111" t="n">
         <v>109</v>
       </c>
       <c r="B111" t="n">
@@ -2326,7 +2331,7 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="1" t="n">
+      <c r="A112" t="n">
         <v>110</v>
       </c>
       <c r="B112" t="n">
@@ -2343,7 +2348,7 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="1" t="n">
+      <c r="A113" t="n">
         <v>111</v>
       </c>
       <c r="B113" t="n">
@@ -2360,7 +2365,7 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="1" t="n">
+      <c r="A114" t="n">
         <v>112</v>
       </c>
       <c r="B114" t="n">
@@ -2377,7 +2382,7 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="1" t="n">
+      <c r="A115" t="n">
         <v>113</v>
       </c>
       <c r="B115" t="n">
@@ -2394,7 +2399,7 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="1" t="n">
+      <c r="A116" t="n">
         <v>114</v>
       </c>
       <c r="B116" t="n">
@@ -2411,7 +2416,7 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="1" t="n">
+      <c r="A117" t="n">
         <v>115</v>
       </c>
       <c r="B117" t="n">
@@ -2428,7 +2433,7 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="1" t="n">
+      <c r="A118" t="n">
         <v>116</v>
       </c>
       <c r="B118" t="n">
@@ -2445,7 +2450,7 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="1" t="n">
+      <c r="A119" t="n">
         <v>117</v>
       </c>
       <c r="B119" t="n">
@@ -2462,7 +2467,7 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="1" t="n">
+      <c r="A120" t="n">
         <v>118</v>
       </c>
       <c r="B120" t="n">
@@ -2479,7 +2484,7 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="1" t="n">
+      <c r="A121" t="n">
         <v>119</v>
       </c>
       <c r="B121" t="n">
@@ -2496,7 +2501,7 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="1" t="n">
+      <c r="A122" t="n">
         <v>120</v>
       </c>
       <c r="B122" t="n">
@@ -2513,7 +2518,7 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="1" t="n">
+      <c r="A123" t="n">
         <v>121</v>
       </c>
       <c r="B123" t="n">
@@ -2530,7 +2535,7 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="1" t="n">
+      <c r="A124" t="n">
         <v>122</v>
       </c>
       <c r="B124" t="n">
@@ -2547,7 +2552,7 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="1" t="n">
+      <c r="A125" t="n">
         <v>123</v>
       </c>
       <c r="B125" t="n">
@@ -2564,7 +2569,7 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="1" t="n">
+      <c r="A126" t="n">
         <v>124</v>
       </c>
       <c r="B126" t="n">
@@ -2581,7 +2586,7 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="1" t="n">
+      <c r="A127" t="n">
         <v>125</v>
       </c>
       <c r="B127" t="n">
@@ -2598,7 +2603,7 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="1" t="n">
+      <c r="A128" t="n">
         <v>126</v>
       </c>
       <c r="B128" t="n">
@@ -2615,7 +2620,7 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="1" t="n">
+      <c r="A129" t="n">
         <v>127</v>
       </c>
       <c r="B129" t="n">
@@ -2632,7 +2637,7 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="1" t="n">
+      <c r="A130" t="n">
         <v>128</v>
       </c>
       <c r="B130" t="n">
@@ -2649,7 +2654,7 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="1" t="n">
+      <c r="A131" t="n">
         <v>129</v>
       </c>
       <c r="B131" t="n">
@@ -2666,7 +2671,7 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="1" t="n">
+      <c r="A132" t="n">
         <v>130</v>
       </c>
       <c r="B132" t="n">
@@ -2683,7 +2688,7 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" s="1" t="n">
+      <c r="A133" t="n">
         <v>131</v>
       </c>
       <c r="B133" t="n">
@@ -2700,7 +2705,7 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" s="1" t="n">
+      <c r="A134" t="n">
         <v>132</v>
       </c>
       <c r="B134" t="n">
@@ -2717,7 +2722,7 @@
       </c>
     </row>
     <row r="135">
-      <c r="A135" s="1" t="n">
+      <c r="A135" t="n">
         <v>133</v>
       </c>
       <c r="B135" t="n">
@@ -2734,7 +2739,7 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" s="1" t="n">
+      <c r="A136" t="n">
         <v>134</v>
       </c>
       <c r="B136" t="n">
@@ -2751,7 +2756,7 @@
       </c>
     </row>
     <row r="137">
-      <c r="A137" s="1" t="n">
+      <c r="A137" t="n">
         <v>135</v>
       </c>
       <c r="B137" t="n">
@@ -2768,7 +2773,7 @@
       </c>
     </row>
     <row r="138">
-      <c r="A138" s="1" t="n">
+      <c r="A138" t="n">
         <v>136</v>
       </c>
       <c r="B138" t="n">
@@ -2785,7 +2790,7 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="1" t="n">
+      <c r="A139" t="n">
         <v>137</v>
       </c>
       <c r="B139" t="n">
@@ -2802,7 +2807,7 @@
       </c>
     </row>
     <row r="140">
-      <c r="A140" s="1" t="n">
+      <c r="A140" t="n">
         <v>138</v>
       </c>
       <c r="B140" t="n">
@@ -2819,7 +2824,7 @@
       </c>
     </row>
     <row r="141">
-      <c r="A141" s="1" t="n">
+      <c r="A141" t="n">
         <v>139</v>
       </c>
       <c r="B141" t="n">
@@ -2836,7 +2841,7 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" s="1" t="n">
+      <c r="A142" t="n">
         <v>140</v>
       </c>
       <c r="B142" t="n">
@@ -2853,7 +2858,7 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" s="1" t="n">
+      <c r="A143" t="n">
         <v>141</v>
       </c>
       <c r="B143" t="n">
@@ -2870,7 +2875,7 @@
       </c>
     </row>
     <row r="144">
-      <c r="A144" s="1" t="n">
+      <c r="A144" t="n">
         <v>142</v>
       </c>
       <c r="B144" t="n">
@@ -2887,7 +2892,7 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="1" t="n">
+      <c r="A145" t="n">
         <v>143</v>
       </c>
       <c r="B145" t="n">
@@ -2904,18 +2909,16 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" s="1" t="n">
-        <v>144</v>
-      </c>
+      <c r="A146" t="inlineStr"/>
       <c r="B146" t="inlineStr"/>
       <c r="C146" t="n">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D146" t="n">
-        <v>0.93</v>
+        <v>0.8</v>
       </c>
       <c r="E146" t="n">
-        <v>0.93</v>
+        <v>1.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>